<commit_message>
Deployed b719260 to develop with MkDocs 1.2.3 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evetion/code/HYDROLIB-core/docs/topics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEEB695-A4A8-944E-9BA7-BCE936065D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14E0B8-ED43-41CA-A6C0-24DACCBE3FC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -30,10 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="133">
   <si>
     <t>Functionality</t>
   </si>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
+  </si>
+  <si>
+    <t>Storage node file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.storagenode.models</t>
+  </si>
+  <si>
+    <t>StorageNodeModel</t>
   </si>
 </sst>
 </file>
@@ -799,12 +805,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -824,7 +830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A2)," ",'Source table'!A2)</f>
         <v>**DIMR**</v>
@@ -850,7 +856,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A3)," ",'Source table'!A3)</f>
         <v>`dimr_config.xml`</v>
@@ -876,7 +882,7 @@
         <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A4)," ",'Source table'!A4)</f>
         <v>FM component</v>
@@ -902,7 +908,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A5)," ",'Source table'!A5)</f>
         <v>RR component</v>
@@ -928,7 +934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A6)," ",'Source table'!A6)</f>
         <v>RTC component</v>
@@ -954,7 +960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A7)," ",'Source table'!A7)</f>
         <v>parallel MPI models</v>
@@ -980,7 +986,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A8)," ",'Source table'!A8)</f>
         <v>coupler elements</v>
@@ -1008,27 +1014,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0CF6A0-E039-4E9E-A3D4-429B45288E31}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,158 +1055,132 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
-        <v>0.1.5</v>
-      </c>
-      <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
-      </c>
-      <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
-        <v>Rainfall .bui file</v>
-      </c>
-      <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="D4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v>0.1.5</v>
       </c>
-      <c r="E4" s="3" t="str">
+      <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
-      </c>
-      <c r="F4" s="3" t="str">
+        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
+      </c>
+      <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <v>Rainfall .bui file</v>
+      </c>
+      <c r="B4" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <v>0.1.5</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <v>_Moved to io.rr in 0.1.6_</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
-        <v>0.1.6*</v>
-      </c>
-      <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
-        <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
-      </c>
-      <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
-        <v>Link file 3b_link.tp</v>
-      </c>
-      <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="D7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v>0.1.6*</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E6" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
-        <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
-      </c>
-      <c r="F7" s="3" t="str">
+        <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
+      </c>
+      <c r="F6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -1218,9 +1199,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A10)," ",'Source table'!A10)</f>
         <v>**FM**</v>
@@ -1266,7 +1247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A11)," ",'Source table'!A11)</f>
         <v>MDU file</v>
@@ -1292,7 +1273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A12)," ",'Source table'!A12)</f>
         <v>Network file `_net.nc`</v>
@@ -1318,7 +1299,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A13)," ",'Source table'!A13)</f>
         <v>**Structure file**</v>
@@ -1344,7 +1325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A14)," ",'Source table'!A14)</f>
         <v>* Weir</v>
@@ -1370,7 +1351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A15)," ",'Source table'!A15)</f>
         <v>* Universal weir</v>
@@ -1396,7 +1377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A16)," ",'Source table'!A16)</f>
         <v>* Culvert</v>
@@ -1422,7 +1403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A17)," ",'Source table'!A17)</f>
         <v>* Long culvert</v>
@@ -1448,7 +1429,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A18)," ",'Source table'!A18)</f>
         <v>* Bridge</v>
@@ -1474,7 +1455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A19)," ",'Source table'!A19)</f>
         <v>* Pump</v>
@@ -1500,7 +1481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A20)," ",'Source table'!A20)</f>
         <v>* Orifice</v>
@@ -1526,7 +1507,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A21)," ",'Source table'!A21)</f>
         <v>* Gate</v>
@@ -1552,7 +1533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A22)," ",'Source table'!A22)</f>
         <v>* General structure</v>
@@ -1578,7 +1559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A23)," ",'Source table'!A23)</f>
         <v>* Dambreak</v>
@@ -1604,7 +1585,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A24)," ",'Source table'!A24)</f>
         <v>* Compound structure</v>
@@ -1630,7 +1611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A25)," ",'Source table'!A25)</f>
         <v>External forcings file (old)</v>
@@ -1656,7 +1637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A26)," ",'Source table'!A26)</f>
         <v>**External forcings file (new)**</v>
@@ -1682,7 +1663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A27)," ",'Source table'!A27)</f>
         <v>* Boundary</v>
@@ -1708,7 +1689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A28)," ",'Source table'!A28)</f>
         <v>* Lateral</v>
@@ -1734,7 +1715,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A29)," ",'Source table'!A29)</f>
         <v>* Meteo</v>
@@ -1760,7 +1741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A30)," ",'Source table'!A30)</f>
         <v>* .bc file</v>
@@ -1786,7 +1767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
         <v>**Cross section files**</v>
@@ -1812,7 +1793,7 @@
         <v>_Moved to io.crosssections in 0.1.6._</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
         <v>Cross section definition file</v>
@@ -1838,7 +1819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
         <v>* Circle</v>
@@ -1864,7 +1845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
         <v>* Rectangle</v>
@@ -1890,7 +1871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
         <v>* Tabulated river</v>
@@ -1916,7 +1897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
         <v>* ZW (tabulated)</v>
@@ -1942,7 +1923,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
         <v>* XYZ</v>
@@ -1968,7 +1949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>* YZ</v>
@@ -1994,7 +1975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section location file</v>
@@ -2020,7 +2001,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>1D roughness file</v>
@@ -2046,44 +2027,44 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
-        <v>**Output**</v>
+        <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.1.6*</v>
       </c>
       <c r="E33" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
-        <v>Observation station file (old)</v>
+        <v>**Output**</v>
       </c>
       <c r="B34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
@@ -2098,18 +2079,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
-        <v>Observation station file (new)</v>
+        <v>Observation station file (old)</v>
       </c>
       <c r="B35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
@@ -2124,18 +2105,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
-        <v>Observation crosssection file (old)</v>
+        <v>Observation station file (new)</v>
       </c>
       <c r="B36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
@@ -2150,18 +2131,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
-        <v>Observation crosssection file (new)</v>
+        <v>Observation crosssection file (old)</v>
       </c>
       <c r="B37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
@@ -2176,10 +2157,10 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
-        <v>History file `_his.nc`</v>
+        <v>Observation crosssection file (new)</v>
       </c>
       <c r="B38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2202,18 +2183,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
-        <v>Map file (old)</v>
+        <v>History file `_his.nc`</v>
       </c>
       <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
@@ -2228,18 +2209,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
-        <v>Map file (UGRID) `_map.nc`</v>
+        <v>Map file (old)</v>
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
@@ -2254,18 +2235,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
-        <v>Fourier input file</v>
+        <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
@@ -2280,18 +2261,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
-        <v>Fourier output file `_fou.nc`</v>
+        <v>Fourier input file</v>
       </c>
       <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
@@ -2303,13 +2284,13 @@
       </c>
       <c r="F42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
-        <v>_via map file reader_</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
-        <v>Class map file</v>
+        <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2332,18 +2313,18 @@
         <v>_via map file reader_</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
-        <v xml:space="preserve"> </v>
+        <v>Class map file</v>
       </c>
       <c r="B44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
@@ -2355,33 +2336,34 @@
       </c>
       <c r="F44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
-        <v xml:space="preserve"> </v>
+        <v>_via map file reader_</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2404,12 +2386,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2432,7 +2414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2452,7 +2434,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2472,7 +2454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2486,7 +2468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2506,7 +2488,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2526,12 +2508,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2551,7 +2533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2571,7 +2553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2591,7 +2573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2611,7 +2593,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2631,7 +2613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2651,7 +2633,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2662,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2682,7 +2664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2702,7 +2684,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2722,7 +2704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2735,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2773,7 +2755,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2793,7 +2775,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +2786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -2824,7 +2806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2844,7 +2826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2864,7 +2846,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2875,7 +2857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2895,7 +2877,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2909,7 +2891,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2929,7 +2911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2949,7 +2931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -2969,7 +2951,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2989,7 +2971,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -3009,7 +2991,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -3029,7 +3011,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -3049,7 +3031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3069,7 +3051,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -3089,58 +3071,67 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>103</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>11</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>105</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>106</v>
-      </c>
-      <c r="B45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>107</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -3149,56 +3140,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>109</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>110</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>111</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>113</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3210,37 +3198,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>115</v>
-      </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>57</v>
-      </c>
-      <c r="E54" t="s">
-        <v>117</v>
-      </c>
-      <c r="F54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>118</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -3252,43 +3231,46 @@
         <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" t="s">
+        <v>120</v>
+      </c>
+      <c r="G56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>122</v>
-      </c>
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" t="s">
-        <v>124</v>
-      </c>
-      <c r="F57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -3303,6 +3285,26 @@
         <v>124</v>
       </c>
       <c r="F58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3321,13 +3323,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3371,7 +3373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Deployed 2116d27 to develop with MkDocs 1.2.3 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14E0B8-ED43-41CA-A6C0-24DACCBE3FC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FFE0C-6B07-4B7A-8BB1-43AFDDF35353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="143">
   <si>
     <t>Functionality</t>
   </si>
@@ -428,6 +428,36 @@
   </si>
   <si>
     <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
+  </si>
+  <si>
+    <t>Initial and parameter field file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.inifield.models</t>
+  </si>
+  <si>
+    <t>IniFieldModel</t>
+  </si>
+  <si>
+    <t>Sample file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.xyz.models</t>
+  </si>
+  <si>
+    <t>XYZModel</t>
+  </si>
+  <si>
+    <t>1D field INI files</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.onedfield.models</t>
+  </si>
+  <si>
+    <t>OneDFieldModel</t>
+  </si>
+  <si>
+    <t>**Spatial data files**</t>
   </si>
   <si>
     <t>Storage node file</t>
@@ -807,7 +837,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,16 +1048,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0CF6A0-E039-4E9E-A3D4-429B45288E31}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,131 +1091,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v>0.1.6*</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <v>Link file 3b_link.tp</v>
+      </c>
+      <c r="B7" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <v>0.1.6*</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1193,13 +1253,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -2029,328 +2095,406 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
-        <v>Storage node file</v>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <v>**Spatial data files**</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
-        <v>0.1.6*</v>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
-        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
-        <v>**Output**</v>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <v>Initial and parameter field file</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <v>0.1.6*</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
-        <v>Observation station file (old)</v>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <v>1D field INI files</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <v>0.1.6*</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
-        <v>Observation station file (new)</v>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <v>Sample file</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <v>0.1.1</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
-        <v>Observation crosssection file (old)</v>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <v>**Output**</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
-        <v>Observation crosssection file (new)</v>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <v>Observation station file (old)</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
-        <v>History file `_his.nc`</v>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <v>Observation station file (new)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
-        <v>Map file (old)</v>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <v>Observation crosssection file (old)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
-        <v>Map file (UGRID) `_map.nc`</v>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <v>Observation crosssection file (new)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
-        <v>Fourier input file</v>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <v>History file `_his.nc`</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
-        <v>Fourier output file `_fou.nc`</v>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <v>Map file (old)</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
-        <v>_via map file reader_</v>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <v>Map file (UGRID) `_map.nc`</v>
+      </c>
+      <c r="B44" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C44" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E44" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F44" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <v>Fourier input file</v>
+      </c>
+      <c r="B45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="C45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E45" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <v>Fourier output file `_fou.nc`</v>
+      </c>
+      <c r="B46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <v>_via map file reader_</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Class map file</v>
       </c>
-      <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+      <c r="B47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+      <c r="C47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E44" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,7 +3217,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3085,108 +3229,129 @@
         <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3194,122 +3359,166 @@
       <c r="C51" t="s">
         <v>11</v>
       </c>
-      <c r="G51" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E59" t="s">
+        <v>117</v>
+      </c>
+      <c r="F59" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" t="s">
+        <v>124</v>
+      </c>
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>125</v>
       </c>
-      <c r="B59" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
         <v>58</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E63" t="s">
         <v>124</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F63" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G58" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G59" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Deployed ce14627 to develop with MkDocs 1.2.3 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FFE0C-6B07-4B7A-8BB1-43AFDDF35353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DE795-08E2-4835-AD20-F6D8D3171D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>0.1.5</t>
   </si>
   <si>
-    <t>0.1.6*</t>
-  </si>
-  <si>
     <t>UniversalWeir</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Cross section location file</t>
   </si>
   <si>
-    <t>Moved to io.crosssections in 0.1.6.</t>
-  </si>
-  <si>
     <t>hydrolib.core.io.crosssection.models</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
     <t>BuiModel</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.1.6</t>
-  </si>
-  <si>
     <t>Node file 3b_node.tp</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>**RR**</t>
   </si>
   <si>
-    <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
-  </si>
-  <si>
     <t>Initial and parameter field file</t>
   </si>
   <si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>StorageNodeModel</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.crosssections in 0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.rr in 0.2.0</t>
+  </si>
+  <si>
+    <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D3)," ",'Source table'!D3)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E3),ISBLANK('Source table'!F3))," ","["&amp;'Source table'!F3&amp;"]["&amp;'Source table'!E3&amp;"."&amp;'Source table'!F3&amp;"]")</f>
@@ -913,7 +913,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G3)," ","_"&amp;'Source table'!G3&amp;"_")</f>
-        <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
+        <v>_Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127)._</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D22)," ",'Source table'!D22)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E14" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E22),ISBLANK('Source table'!F22))," ","["&amp;'Source table'!F22&amp;"]["&amp;'Source table'!E22&amp;"."&amp;'Source table'!F22&amp;"]")</f>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="F23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
-        <v>_Moved to io.crosssections in 0.1.6._</v>
+        <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="D32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2546,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2555,7 +2555,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -2754,7 +2754,7 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
         <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2870,13 +2870,13 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,12 +2916,12 @@
         <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -2944,15 +2944,15 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
-      </c>
-      <c r="F26" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -2964,15 +2964,15 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -2984,15 +2984,15 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3015,15 +3015,15 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3032,12 +3032,12 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3049,15 +3049,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" t="s">
         <v>80</v>
-      </c>
-      <c r="F32" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3069,15 +3069,15 @@
         <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3089,15 +3089,15 @@
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3109,15 +3109,15 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3129,15 +3129,15 @@
         <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3149,15 +3149,15 @@
         <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3169,15 +3169,15 @@
         <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3189,35 +3189,35 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
-      <c r="F40" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3226,23 +3226,23 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -3251,18 +3251,18 @@
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -3271,18 +3271,18 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3294,20 +3294,20 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -3404,12 +3404,12 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -3418,17 +3418,17 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
@@ -3440,18 +3440,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3463,23 +3463,23 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G60" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -3488,18 +3488,18 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -3508,13 +3508,13 @@
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
         <v>124</v>
-      </c>
-      <c r="F63" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed cac9441 to develop with MkDocs 1.2.3 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DE795-08E2-4835-AD20-F6D8D3171D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DCA94-3F1A-4A7C-906F-C037CFB44E1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -1253,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,390 +2095,416 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <v>Storage node file</v>
+      </c>
+      <c r="B33" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C33" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <v>0.2.0</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>**Spatial data files**</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C33" t="str">
+      <c r="C34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E33" s="3" t="str">
+      <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F33" s="3" t="str">
+      <c r="F34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="str">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>Initial and parameter field file</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.2.0</v>
       </c>
-      <c r="E34" s="3" t="str">
+      <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
-      <c r="F34" s="3" t="str">
+      <c r="F35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="str">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>1D field INI files</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.2.0</v>
       </c>
-      <c r="E35" s="3" t="str">
+      <c r="E36" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
-      <c r="F35" s="3" t="str">
+      <c r="F36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="str">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>Sample file</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.1</v>
       </c>
-      <c r="E36" s="3" t="str">
+      <c r="E37" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
-      <c r="F36" s="3" t="str">
+      <c r="F37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="str">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>**Output**</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C37" t="str">
+      <c r="C38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E37" s="3" t="str">
+      <c r="E38" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F37" s="3" t="str">
+      <c r="F38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="str">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>Observation station file (old)</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E38" s="3" t="str">
+      <c r="E39" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F38" s="3" t="str">
+      <c r="F39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="str">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Observation station file (new)</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E39" s="3" t="str">
+      <c r="E40" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F39" s="3" t="str">
+      <c r="F40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="str">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>Observation crosssection file (old)</v>
       </c>
-      <c r="B40" t="str">
+      <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E40" s="3" t="str">
+      <c r="E41" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F40" s="3" t="str">
+      <c r="F41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="str">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Observation crosssection file (new)</v>
       </c>
-      <c r="B41" t="str">
+      <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E41" s="3" t="str">
+      <c r="E42" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F41" s="3" t="str">
+      <c r="F42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="str">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>History file `_his.nc`</v>
       </c>
-      <c r="B42" t="str">
+      <c r="B43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C42" t="str">
+      <c r="C43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E42" s="3" t="str">
+      <c r="E43" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F42" s="3" t="str">
+      <c r="F43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="str">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Map file (old)</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E43" s="3" t="str">
+      <c r="E44" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F43" s="3" t="str">
+      <c r="F44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="str">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
-      <c r="B44" t="str">
+      <c r="B45" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C45" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E44" s="3" t="str">
+      <c r="E45" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F44" s="3" t="str">
+      <c r="F45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="str">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Fourier input file</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B46" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C46" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E45" s="3" t="str">
+      <c r="E46" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F45" s="3" t="str">
+      <c r="F46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="str">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
-      <c r="B46" t="str">
+      <c r="B47" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C47" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E46" s="3" t="str">
+      <c r="E47" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F46" s="3" t="str">
+      <c r="F47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="str">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Class map file</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B48" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C48" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E47" s="3" t="str">
+      <c r="E48" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F47" s="3" t="str">
+      <c r="F48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
@@ -2493,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deployed a8eecbe to develop with MkDocs 1.3.0 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DCA94-3F1A-4A7C-906F-C037CFB44E1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
   <si>
     <t>Functionality</t>
   </si>
@@ -385,15 +385,9 @@
     <t>RainfallRunoffModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.fnm.models</t>
-  </si>
-  <si>
     <t>Rainfall .bui file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.bui.models</t>
-  </si>
-  <si>
     <t>BuiModel</t>
   </si>
   <si>
@@ -463,10 +457,28 @@
     <t>Moved to io.crosssections in 0.2.0</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.2.0</t>
-  </si>
-  <si>
     <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obs.models</t>
+  </si>
+  <si>
+    <t>ObservationPointModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.models</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.fnm.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.bui.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.meteo.models</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1146,11 @@
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
+        <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,11 +1172,11 @@
       </c>
       <c r="E4" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
+        <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,7 +1268,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,19 +2294,19 @@
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
@@ -2519,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2584,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2581,7 +2593,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -3058,7 +3070,7 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3232,7 +3244,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
         <v>95</v>
@@ -3243,72 +3255,72 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" t="s">
         <v>126</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>139</v>
-      </c>
-      <c r="E43" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" t="s">
         <v>132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>139</v>
-      </c>
-      <c r="E44" t="s">
-        <v>133</v>
-      </c>
-      <c r="F44" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3320,10 +3332,10 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3347,10 +3359,19 @@
         <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,7 +3470,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3466,18 +3487,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
         <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3489,58 +3510,58 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="F60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" t="s">
         <v>119</v>
       </c>
-      <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>121</v>
-      </c>
-      <c r="F62" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+      <c r="E63" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" t="s">
         <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed 39fe154 to develop with MkDocs 1.3.0 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/develop/topics/dhydro_support_hydrolib-core.xlsx
+++ b/develop/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17C55D-05C7-4B4E-ADB6-65EACAF64AA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Functionality</t>
   </si>
@@ -479,6 +479,57 @@
   </si>
   <si>
     <t>hydrolib.core.io.rr.meteo.models</t>
+  </si>
+  <si>
+    <t>** timeSeries</t>
+  </si>
+  <si>
+    <t>** harmonic (-Correction)</t>
+  </si>
+  <si>
+    <t>** astronomic (-Correction)</t>
+  </si>
+  <si>
+    <t>** t3D</t>
+  </si>
+  <si>
+    <t>** QHTable</t>
+  </si>
+  <si>
+    <t>** constant</t>
+  </si>
+  <si>
+    <t>** vector quantities</t>
+  </si>
+  <si>
+    <t>TimeSeries</t>
+  </si>
+  <si>
+    <t>T3D</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>0.3.1</t>
+  </si>
+  <si>
+    <t>VectorQuantityUnitPairs</t>
+  </si>
+  <si>
+    <t>QHTable</t>
+  </si>
+  <si>
+    <t>Astronomic</t>
+  </si>
+  <si>
+    <t>Harmonic</t>
+  </si>
+  <si>
+    <t>ObservationCrossSectionModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obscrosssection.models</t>
   </si>
 </sst>
 </file>
@@ -844,7 +895,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,157 +1154,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A65)," ",'Source table'!A65)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D65)," ",'Source table'!D65)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E65),ISBLANK('Source table'!F65))," ","["&amp;'Source table'!F65&amp;"]["&amp;'Source table'!E65&amp;"."&amp;'Source table'!F65&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G65)," ","_"&amp;'Source table'!G65&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
+        <f>IF(ISBLANK('Source table'!A66)," ",'Source table'!A66)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
+        <f>IF(ISBLANK('Source table'!D66)," ",'Source table'!D66)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E66),ISBLANK('Source table'!F66))," ","["&amp;'Source table'!F66&amp;"]["&amp;'Source table'!E66&amp;"."&amp;'Source table'!F66&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G66)," ","_"&amp;'Source table'!G66&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
+        <f>IF(ISBLANK('Source table'!A67)," ",'Source table'!A67)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
+        <f>IF(ISBLANK('Source table'!D67)," ",'Source table'!D67)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
+        <f>IF(ISBLANK('Source table'!A68)," ",'Source table'!A68)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
+        <f>IF(ISBLANK('Source table'!D68)," ",'Source table'!D68)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E68),ISBLANK('Source table'!F68))," ","["&amp;'Source table'!F68&amp;"]["&amp;'Source table'!E68&amp;"."&amp;'Source table'!F68&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G68)," ","_"&amp;'Source table'!G68&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
+        <f>IF(ISBLANK('Source table'!A69)," ",'Source table'!A69)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
+        <f>IF(ISBLANK('Source table'!D69)," ",'Source table'!D69)</f>
         <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <f>IF(ISBLANK('Source table'!A70)," ",'Source table'!A70)</f>
         <v>Link file 3b_link.tp</v>
       </c>
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <f>IF(ISBLANK('Source table'!D70)," ",'Source table'!D70)</f>
         <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
         <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1267,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,677 +1898,677 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
+        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>**Cross section files**</v>
       </c>
       <c r="B23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D31)," ",'Source table'!D31)</f>
+        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E31),ISBLANK('Source table'!F31))," ","["&amp;'Source table'!F31&amp;"]["&amp;'Source table'!E31&amp;"."&amp;'Source table'!F31&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
         <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
+        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section definition file</v>
       </c>
       <c r="B24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D32)," ",'Source table'!D32)</f>
+        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
         <v>0.1.1</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E32),ISBLANK('Source table'!F32))," ","["&amp;'Source table'!F32&amp;"]["&amp;'Source table'!E32&amp;"."&amp;'Source table'!F32&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
         <v>[CrossDefModel][hydrolib.core.io.crosssection.models.CrossDefModel]</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G32)," ","_"&amp;'Source table'!G32&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
+        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>* Circle</v>
       </c>
       <c r="B25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D33)," ",'Source table'!D33)</f>
+        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
         <v>0.1.5</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E33),ISBLANK('Source table'!F33))," ","["&amp;'Source table'!F33&amp;"]["&amp;'Source table'!E33&amp;"."&amp;'Source table'!F33&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
         <v>[CircleCrsDef][hydrolib.core.io.crosssection.models.CircleCrsDef]</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G33)," ","_"&amp;'Source table'!G33&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
         <v>* Rectangle</v>
       </c>
       <c r="B26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D34)," ",'Source table'!D34)</f>
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
         <v>0.1.5</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E34),ISBLANK('Source table'!F34))," ","["&amp;'Source table'!F34&amp;"]["&amp;'Source table'!E34&amp;"."&amp;'Source table'!F34&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
         <v>[RectangleCrsDef][hydrolib.core.io.crosssection.models.RectangleCrsDef]</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G34)," ","_"&amp;'Source table'!G34&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>* Tabulated river</v>
       </c>
       <c r="B27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D35)," ",'Source table'!D35)</f>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v>0.1.5</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E35),ISBLANK('Source table'!F35))," ","["&amp;'Source table'!F35&amp;"]["&amp;'Source table'!E35&amp;"."&amp;'Source table'!F35&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v>[ZWRiverCrsDef][hydrolib.core.io.crosssection.models.ZWRiverCrsDef]</v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G35)," ","_"&amp;'Source table'!G35&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>* ZW (tabulated)</v>
       </c>
       <c r="B28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D36)," ",'Source table'!D36)</f>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.1.5</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E36),ISBLANK('Source table'!F36))," ","["&amp;'Source table'!F36&amp;"]["&amp;'Source table'!E36&amp;"."&amp;'Source table'!F36&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[ZWCrsDef][hydrolib.core.io.crosssection.models.ZWCrsDef]</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G36)," ","_"&amp;'Source table'!G36&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>* XYZ</v>
       </c>
       <c r="B29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D37)," ",'Source table'!D37)</f>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.1.5</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E37),ISBLANK('Source table'!F37))," ","["&amp;'Source table'!F37&amp;"]["&amp;'Source table'!E37&amp;"."&amp;'Source table'!F37&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[XYZCrsDef][hydrolib.core.io.crosssection.models.XYZCrsDef]</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G37)," ","_"&amp;'Source table'!G37&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>* YZ</v>
       </c>
       <c r="B30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.5</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[YZCrsDef][hydrolib.core.io.crosssection.models.YZCrsDef]</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>Cross section location file</v>
       </c>
       <c r="B31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v>0.1.1</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v>[CrossLocModel][hydrolib.core.io.crosssection.models.CrossLocModel]</v>
       </c>
       <c r="F31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>1D roughness file</v>
       </c>
       <c r="B32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v>[FrictionModel][hydrolib.core.io.friction.models.FrictionModel]</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v>0.2.0</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>**Spatial data files**</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Initial and parameter field file</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>1D field INI files</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v>0.2.0</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Sample file</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v>0.1.1</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>**Output**</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Observation station file (old)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Observation station file (new)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Observation crosssection file (old)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>Observation crosssection file (new)</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <v>0.3.1</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <v>[ObservationCrossSectionModel][hydrolib.core.io.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>History file `_his.nc`</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Map file (old)</v>
       </c>
       <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>Fourier input file</v>
       </c>
       <c r="B46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E47" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
         <v>Class map file</v>
       </c>
       <c r="B48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E48" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
@@ -2529,10 +2580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,7 +2866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2826,7 +2877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2846,7 +2897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2886,7 +2937,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2897,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2917,7 +2968,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2937,7 +2988,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2968,7 +3019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2988,7 +3039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3008,7 +3059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -3028,7 +3079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3039,7 +3090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -3059,9 +3110,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3069,13 +3120,19 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3087,15 +3144,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3104,18 +3161,18 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3124,18 +3181,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3144,18 +3201,18 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3164,18 +3221,18 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3184,18 +3241,18 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3203,19 +3260,13 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3230,208 +3281,262 @@
         <v>78</v>
       </c>
       <c r="F39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
         <v>137</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E47" t="s">
         <v>95</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>134</v>
       </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>137</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E48" t="s">
         <v>135</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F48" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3442,132 +3547,227 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
-        <v>110</v>
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>110</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E59" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" t="s">
-        <v>144</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
-        <v>57</v>
-      </c>
-      <c r="E60" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" t="s">
-        <v>116</v>
-      </c>
-      <c r="G60" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>137</v>
-      </c>
-      <c r="E62" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" t="s">
-        <v>121</v>
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" t="s">
+        <v>114</v>
+      </c>
+      <c r="G66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>120</v>
       </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>137</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>119</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F70" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G59" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G70" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>